<commit_message>
SU maj front upper A-Arm
</commit_message>
<xml_diff>
--- a/SU_Suspension/Parametres.xlsx
+++ b/SU_Suspension/Parametres.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>bracket_e (mm)</t>
   </si>
@@ -54,6 +54,18 @@
   </si>
   <si>
     <t>shim_e (mm)</t>
+  </si>
+  <si>
+    <t>insert_a (mm)</t>
+  </si>
+  <si>
+    <t>insert_b (mm)</t>
+  </si>
+  <si>
+    <t>insert_c (mm)</t>
+  </si>
+  <si>
+    <t>insert_r (mm)</t>
   </si>
 </sst>
 </file>
@@ -109,6 +121,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>597864</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>10306</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Immagine 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5255589" y="914400"/>
+          <a:ext cx="3126411" cy="2715406"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -374,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,8 +523,41 @@
         <v>7</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SU maj lower rear A-Arm
</commit_message>
<xml_diff>
--- a/SU_Suspension/Parametres.xlsx
+++ b/SU_Suspension/Parametres.xlsx
@@ -432,7 +432,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +544,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
SU maj Rear Upright
hail Upright
</commit_message>
<xml_diff>
--- a/SU_Suspension/Parametres.xlsx
+++ b/SU_Suspension/Parametres.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>bracket_e (mm)</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>insert_r (mm)</t>
+  </si>
+  <si>
+    <t>Rcaliper_offset (mm)</t>
+  </si>
+  <si>
+    <t>Rcaliper_radius (mm)</t>
+  </si>
+  <si>
+    <t>Rcaliper_distance (mm)</t>
   </si>
 </sst>
 </file>
@@ -429,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +496,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -553,6 +562,30 @@
       </c>
       <c r="B14" s="2">
         <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SU front Upright coming
</commit_message>
<xml_diff>
--- a/SU_Suspension/Parametres.xlsx
+++ b/SU_Suspension/Parametres.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>bracket_e (mm)</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>Rcaliper_distance (mm)</t>
+  </si>
+  <si>
+    <t>Fcaliper_offset (mm)</t>
+  </si>
+  <si>
+    <t>Fcaliper_radius (mm)</t>
+  </si>
+  <si>
+    <t>Fcaliper_distance (mm)</t>
   </si>
 </sst>
 </file>
@@ -438,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,6 +597,30 @@
         <v>84</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>69.849999999999994</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
SU maj position Rear Caliper
</commit_message>
<xml_diff>
--- a/SU_Suspension/Parametres.xlsx
+++ b/SU_Suspension/Parametres.xlsx
@@ -450,7 +450,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +578,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -586,7 +586,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>